<commit_message>
update order thiết kế
</commit_message>
<xml_diff>
--- a/Bao_cao/Thiết kế/Thiết kế chi tiết/MILKTEAMANAGEMENT_TLPT_02_Order.xlsx
+++ b/Bao_cao/Thiết kế/Thiết kế chi tiết/MILKTEAMANAGEMENT_TLPT_02_Order.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9024" tabRatio="826" activeTab="1"/>
+    <workbookView windowWidth="22188" windowHeight="9024" tabRatio="826" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_bìa" sheetId="19" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="237">
   <si>
     <t xml:space="preserve">Posts and Telecommunications Institute of Technology
 </t>
@@ -616,7 +616,16 @@
     <t>Spinner</t>
   </si>
   <si>
+    <t>Chỉ có thể nhập được số nguyên dương</t>
+  </si>
+  <si>
+    <t>Chỉ có thể nhập được số nguyên</t>
+  </si>
+  <si>
     <t>EditText</t>
+  </si>
+  <si>
+    <t>Chỉ có thể nhập được số nguyên &gt; 0</t>
   </si>
   <si>
     <t>[Vùng nút]</t>
@@ -682,7 +691,7 @@
     <t>Sau khi chọn hoàn tất, hiển thị món đã chọn xuống bảng danh sách bên dưới</t>
   </si>
   <si>
-    <t>Thay đổi sub total, grand total</t>
+    <t>Thay đổi sub total += Product.price * quantity</t>
   </si>
   <si>
     <t>(3) Xoá món đã thêm</t>
@@ -697,6 +706,9 @@
     <t>Sau khi xoá thành công thì xoá món ở trong bảng danh sách món</t>
   </si>
   <si>
+    <t>Thay đổi sub total</t>
+  </si>
+  <si>
     <t>(4) Thêm toppings cho món</t>
   </si>
   <si>
@@ -706,7 +718,7 @@
     <t>Sau khi chọn hoàn tất, cập nhận total của món</t>
   </si>
   <si>
-    <t>Thay đổi sub total, grand total theo giá của toppings</t>
+    <t>Thay đổi sub total += Toppings.price</t>
   </si>
   <si>
     <t>(5) Chỉnh sửa size cho món</t>
@@ -718,7 +730,7 @@
     <t>Sau khi chọn, cập nhật total của món</t>
   </si>
   <si>
-    <t>Thay đổi sub total, grand total theo giá của sizes</t>
+    <t>Thay đổi sub total += Size.price</t>
   </si>
   <si>
     <t>(6) Chỉnh sửa sugar cho món</t>
@@ -739,7 +751,7 @@
     <t>Mặc định thuế là 0%, chọn Textview Tax Inclusive chỉnh sửa thuế của món</t>
   </si>
   <si>
-    <t>Thay đổi grand total theo tax hiện tại</t>
+    <t>Thay đổi grand total = sub total + sub total * tax%</t>
   </si>
   <si>
     <t>(9) Hoàn tất order</t>
@@ -30804,8 +30816,8 @@
   <sheetPr/>
   <dimension ref="A1:BF145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="112" zoomScaleNormal="113" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="112" zoomScaleNormal="113" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="Y130" sqref="Y130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.66666666666667" defaultRowHeight="13.5" customHeight="1"/>
@@ -34400,7 +34412,9 @@
       <c r="AA61" s="71"/>
       <c r="AB61" s="71"/>
       <c r="AC61" s="71"/>
-      <c r="AD61" s="91"/>
+      <c r="AD61" s="91" t="s">
+        <v>130</v>
+      </c>
       <c r="AE61" s="71"/>
       <c r="AF61" s="71"/>
       <c r="AG61" s="71"/>
@@ -34466,7 +34480,9 @@
       <c r="AA62" s="75"/>
       <c r="AB62" s="75"/>
       <c r="AC62" s="75"/>
-      <c r="AD62" s="126"/>
+      <c r="AD62" s="126" t="s">
+        <v>131</v>
+      </c>
       <c r="AE62" s="75"/>
       <c r="AF62" s="75"/>
       <c r="AG62" s="75"/>
@@ -34523,7 +34539,7 @@
       </c>
       <c r="U63" s="314"/>
       <c r="V63" s="126" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="W63" s="75"/>
       <c r="X63" s="75"/>
@@ -34532,7 +34548,9 @@
       <c r="AA63" s="75"/>
       <c r="AB63" s="75"/>
       <c r="AC63" s="75"/>
-      <c r="AD63" s="126"/>
+      <c r="AD63" s="126" t="s">
+        <v>133</v>
+      </c>
       <c r="AE63" s="75"/>
       <c r="AF63" s="75"/>
       <c r="AG63" s="75"/>
@@ -34765,7 +34783,7 @@
       <c r="A68" s="59"/>
       <c r="B68" s="258"/>
       <c r="C68" s="62" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D68" s="62"/>
       <c r="E68" s="62"/>
@@ -34937,7 +34955,7 @@
         <v>2</v>
       </c>
       <c r="D71" s="359" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E71" s="360"/>
       <c r="F71" s="360"/>
@@ -34949,7 +34967,7 @@
       <c r="L71" s="360"/>
       <c r="M71" s="380"/>
       <c r="N71" s="360" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="O71" s="360"/>
       <c r="P71" s="360"/>
@@ -34994,7 +35012,7 @@
         <v>3</v>
       </c>
       <c r="D72" s="359" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E72" s="360"/>
       <c r="F72" s="360"/>
@@ -35006,7 +35024,7 @@
       <c r="L72" s="360"/>
       <c r="M72" s="380"/>
       <c r="N72" s="360" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="O72" s="360"/>
       <c r="P72" s="360"/>
@@ -35063,7 +35081,7 @@
       <c r="L73" s="360"/>
       <c r="M73" s="380"/>
       <c r="N73" s="360" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="O73" s="360"/>
       <c r="P73" s="360"/>
@@ -35120,7 +35138,7 @@
       <c r="L74" s="360"/>
       <c r="M74" s="380"/>
       <c r="N74" s="360" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="O74" s="360"/>
       <c r="P74" s="360"/>
@@ -35177,7 +35195,7 @@
       <c r="L75" s="360"/>
       <c r="M75" s="380"/>
       <c r="N75" s="360" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="O75" s="360"/>
       <c r="P75" s="360"/>
@@ -35234,7 +35252,7 @@
       <c r="L76" s="62"/>
       <c r="M76" s="116"/>
       <c r="N76" s="360" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="O76" s="62"/>
       <c r="P76" s="62"/>
@@ -35279,7 +35297,7 @@
         <v>8</v>
       </c>
       <c r="D77" s="363" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E77" s="364"/>
       <c r="F77" s="364"/>
@@ -35291,7 +35309,7 @@
       <c r="L77" s="364"/>
       <c r="M77" s="381"/>
       <c r="N77" s="62" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="O77" s="364"/>
       <c r="P77" s="364"/>
@@ -35751,7 +35769,7 @@
     <row r="85" s="49" customFormat="1" customHeight="1" spans="1:58">
       <c r="A85" s="59"/>
       <c r="B85" s="60" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C85" s="61"/>
       <c r="D85" s="62"/>
@@ -35813,7 +35831,7 @@
       <c r="A86" s="59"/>
       <c r="B86" s="60"/>
       <c r="C86" s="61" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D86" s="62"/>
       <c r="E86" s="62"/>
@@ -35875,7 +35893,7 @@
       <c r="B87" s="60"/>
       <c r="C87" s="61"/>
       <c r="D87" s="581" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="E87" s="62"/>
       <c r="F87" s="62"/>
@@ -35951,7 +35969,7 @@
       <c r="M88" s="89"/>
       <c r="N88" s="114"/>
       <c r="O88" s="89" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="P88" s="89"/>
       <c r="Q88" s="89"/>
@@ -36014,7 +36032,7 @@
       <c r="M89" s="92"/>
       <c r="N89" s="115"/>
       <c r="O89" s="92" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="P89" s="92"/>
       <c r="Q89" s="92"/>
@@ -36077,7 +36095,7 @@
       <c r="M90" s="360"/>
       <c r="N90" s="380"/>
       <c r="O90" s="360" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="P90" s="360"/>
       <c r="Q90" s="360"/>
@@ -36140,7 +36158,7 @@
       <c r="M91" s="360"/>
       <c r="N91" s="380"/>
       <c r="O91" s="360" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="P91" s="360"/>
       <c r="Q91" s="360"/>
@@ -36203,7 +36221,7 @@
       <c r="M92" s="360"/>
       <c r="N92" s="380"/>
       <c r="O92" s="360" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="P92" s="360"/>
       <c r="Q92" s="360"/>
@@ -36266,7 +36284,7 @@
       <c r="M93" s="340"/>
       <c r="N93" s="385"/>
       <c r="O93" s="340" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="P93" s="340"/>
       <c r="Q93" s="340"/>
@@ -36372,7 +36390,7 @@
       <c r="A95" s="59"/>
       <c r="B95" s="60"/>
       <c r="C95" s="61" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D95" s="62"/>
       <c r="E95" s="62"/>
@@ -36434,7 +36452,7 @@
       <c r="B96" s="60"/>
       <c r="C96" s="61"/>
       <c r="D96" s="581" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E96" s="62"/>
       <c r="F96" s="62"/>
@@ -36495,7 +36513,7 @@
       <c r="B97" s="60"/>
       <c r="C97" s="61"/>
       <c r="D97" s="62" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E97" s="62"/>
       <c r="F97" s="62"/>
@@ -36556,7 +36574,7 @@
       <c r="B98" s="60"/>
       <c r="C98" s="61"/>
       <c r="D98" s="62" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E98" s="62"/>
       <c r="F98" s="62"/>
@@ -36617,7 +36635,7 @@
       <c r="B99" s="60"/>
       <c r="C99" s="61"/>
       <c r="D99" s="50" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E99" s="62"/>
       <c r="F99" s="62"/>
@@ -36678,7 +36696,7 @@
       <c r="B100" s="60"/>
       <c r="C100" s="61"/>
       <c r="D100" s="50" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E100" s="62"/>
       <c r="F100" s="62"/>
@@ -36797,7 +36815,7 @@
       <c r="A102" s="59"/>
       <c r="B102" s="60"/>
       <c r="C102" s="61" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D102" s="62"/>
       <c r="E102" s="62"/>
@@ -36859,7 +36877,7 @@
       <c r="B103" s="60"/>
       <c r="C103" s="61"/>
       <c r="D103" s="581" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E103" s="62"/>
       <c r="F103" s="62"/>
@@ -36920,7 +36938,7 @@
       <c r="B104" s="60"/>
       <c r="C104" s="61"/>
       <c r="D104" s="62" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E104" s="62"/>
       <c r="F104" s="62"/>
@@ -36981,7 +36999,7 @@
       <c r="B105" s="60"/>
       <c r="C105" s="61"/>
       <c r="D105" s="62" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E105" s="62"/>
       <c r="F105" s="62"/>
@@ -37042,7 +37060,7 @@
       <c r="B106" s="60"/>
       <c r="C106" s="61"/>
       <c r="D106" s="50" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
       <c r="E106" s="62"/>
       <c r="F106" s="62"/>
@@ -37161,7 +37179,7 @@
       <c r="A108" s="59"/>
       <c r="B108" s="60"/>
       <c r="C108" s="61" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D108" s="62"/>
       <c r="E108" s="62"/>
@@ -37223,7 +37241,7 @@
       <c r="B109" s="60"/>
       <c r="C109" s="61"/>
       <c r="D109" s="62" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E109" s="62"/>
       <c r="F109" s="62"/>
@@ -37284,7 +37302,7 @@
       <c r="B110" s="60"/>
       <c r="C110" s="61"/>
       <c r="D110" s="62" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E110" s="62"/>
       <c r="F110" s="62"/>
@@ -37345,7 +37363,7 @@
       <c r="B111" s="60"/>
       <c r="C111" s="61"/>
       <c r="D111" s="50" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="E111" s="62"/>
       <c r="F111" s="62"/>
@@ -37464,7 +37482,7 @@
       <c r="A113" s="59"/>
       <c r="B113" s="60"/>
       <c r="C113" s="582" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D113" s="62"/>
       <c r="E113" s="62"/>
@@ -37526,7 +37544,7 @@
       <c r="B114" s="60"/>
       <c r="C114" s="61"/>
       <c r="D114" s="62" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="E114" s="62"/>
       <c r="F114" s="62"/>
@@ -37587,7 +37605,7 @@
       <c r="B115" s="60"/>
       <c r="C115" s="61"/>
       <c r="D115" s="62" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E115" s="62"/>
       <c r="F115" s="62"/>
@@ -37648,7 +37666,7 @@
       <c r="B116" s="60"/>
       <c r="C116" s="61"/>
       <c r="D116" s="50" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E116" s="62"/>
       <c r="F116" s="62"/>
@@ -37767,7 +37785,7 @@
       <c r="A118" s="59"/>
       <c r="B118" s="60"/>
       <c r="C118" s="582" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D118" s="62"/>
       <c r="E118" s="62"/>
@@ -37829,7 +37847,7 @@
       <c r="B119" s="60"/>
       <c r="C119" s="61"/>
       <c r="D119" s="62" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="E119" s="62"/>
       <c r="F119" s="62"/>
@@ -37948,7 +37966,7 @@
       <c r="A121" s="59"/>
       <c r="B121" s="60"/>
       <c r="C121" s="582" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D121" s="62"/>
       <c r="E121" s="62"/>
@@ -38010,7 +38028,7 @@
       <c r="B122" s="60"/>
       <c r="C122" s="61"/>
       <c r="D122" s="62" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E122" s="62"/>
       <c r="F122" s="62"/>
@@ -38129,7 +38147,7 @@
       <c r="A124" s="59"/>
       <c r="B124" s="60"/>
       <c r="C124" s="582" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D124" s="62"/>
       <c r="E124" s="62"/>
@@ -38191,7 +38209,7 @@
       <c r="B125" s="60"/>
       <c r="C125" s="61"/>
       <c r="D125" s="62" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E125" s="62"/>
       <c r="F125" s="62"/>
@@ -38252,7 +38270,7 @@
       <c r="B126" s="60"/>
       <c r="C126" s="61"/>
       <c r="D126" s="50" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E126" s="62"/>
       <c r="F126" s="62"/>
@@ -38371,7 +38389,7 @@
       <c r="A128" s="59"/>
       <c r="B128" s="60"/>
       <c r="C128" s="61" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D128" s="62"/>
       <c r="E128" s="62"/>
@@ -38433,7 +38451,7 @@
       <c r="B129" s="60"/>
       <c r="C129" s="61"/>
       <c r="D129" s="62" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E129" s="62"/>
       <c r="F129" s="62"/>
@@ -38494,7 +38512,7 @@
       <c r="B130" s="60"/>
       <c r="C130" s="61"/>
       <c r="D130" s="581" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E130" s="62"/>
       <c r="F130" s="62"/>
@@ -38555,7 +38573,7 @@
       <c r="B131" s="60"/>
       <c r="C131" s="61"/>
       <c r="D131" s="62" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E131" s="62"/>
       <c r="F131" s="62"/>
@@ -38616,7 +38634,7 @@
       <c r="B132" s="60"/>
       <c r="C132" s="61"/>
       <c r="D132" s="581" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E132" s="62"/>
       <c r="F132" s="62"/>
@@ -38677,7 +38695,7 @@
       <c r="B133" s="60"/>
       <c r="C133" s="61"/>
       <c r="D133" s="62" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E133" s="62"/>
       <c r="F133" s="62"/>
@@ -38738,7 +38756,7 @@
       <c r="B134" s="60"/>
       <c r="C134" s="61"/>
       <c r="D134" s="62" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E134" s="62"/>
       <c r="F134" s="62"/>
@@ -39181,7 +39199,7 @@
     <row r="141" s="49" customFormat="1" customHeight="1" spans="1:58">
       <c r="A141" s="59"/>
       <c r="B141" s="60" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C141" s="61"/>
       <c r="D141" s="62"/>
@@ -39243,7 +39261,7 @@
       <c r="A142" s="59"/>
       <c r="B142" s="60"/>
       <c r="C142" s="392" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D142" s="393"/>
       <c r="E142" s="393"/>
@@ -39577,8 +39595,8 @@
   <sheetPr/>
   <dimension ref="A1:BG198"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="113" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:I3"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="113" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="P82" sqref="P82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.66666666666667" defaultRowHeight="13.5" customHeight="1"/>
@@ -39592,7 +39610,7 @@
   <sheetData>
     <row r="1" s="49" customFormat="1" customHeight="1" spans="1:58">
       <c r="A1" s="53" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B1" s="54"/>
       <c r="C1" s="54"/>
@@ -39857,7 +39875,7 @@
     <row r="5" s="49" customFormat="1" customHeight="1" spans="1:58">
       <c r="A5" s="59"/>
       <c r="B5" s="60" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C5" s="61"/>
       <c r="D5" s="62"/>
@@ -39919,7 +39937,7 @@
       <c r="A6" s="59"/>
       <c r="B6" s="60"/>
       <c r="C6" s="61" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D6" s="62"/>
       <c r="E6" s="63"/>
@@ -39973,7 +39991,7 @@
       <c r="B7" s="60"/>
       <c r="C7" s="61"/>
       <c r="D7" s="62" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E7" s="63"/>
       <c r="F7" s="62"/>
@@ -40026,7 +40044,7 @@
       <c r="B8" s="60"/>
       <c r="C8" s="61"/>
       <c r="D8" s="581" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E8" s="64"/>
       <c r="F8" s="62"/>
@@ -41805,7 +41823,7 @@
         <v>1</v>
       </c>
       <c r="E38" s="70" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F38" s="71"/>
       <c r="G38" s="71"/>
@@ -41824,7 +41842,7 @@
       <c r="R38" s="72"/>
       <c r="S38" s="106"/>
       <c r="T38" s="91" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="U38" s="71"/>
       <c r="V38" s="71"/>
@@ -41874,7 +41892,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="74" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F39" s="75"/>
       <c r="G39" s="75"/>
@@ -41893,7 +41911,7 @@
       <c r="R39" s="76"/>
       <c r="S39" s="107"/>
       <c r="T39" s="126" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="U39" s="75"/>
       <c r="V39" s="75"/>
@@ -41943,7 +41961,7 @@
         <v>3</v>
       </c>
       <c r="E40" s="78" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F40" s="79"/>
       <c r="G40" s="79"/>
@@ -41962,7 +41980,7 @@
       <c r="R40" s="80"/>
       <c r="S40" s="108"/>
       <c r="T40" s="78" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="U40" s="79"/>
       <c r="V40" s="79"/>
@@ -42209,7 +42227,7 @@
         <v>1</v>
       </c>
       <c r="E44" s="84" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F44" s="85"/>
       <c r="G44" s="85"/>
@@ -42237,7 +42255,7 @@
       </c>
       <c r="V44" s="132"/>
       <c r="W44" s="84" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="X44" s="85"/>
       <c r="Y44" s="85"/>
@@ -42338,7 +42356,7 @@
       <c r="B46" s="60"/>
       <c r="C46" s="61"/>
       <c r="D46" s="62" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E46" s="62"/>
       <c r="F46" s="62"/>
@@ -42469,7 +42487,7 @@
         <v>1</v>
       </c>
       <c r="E48" s="91" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F48" s="92"/>
       <c r="G48" s="92"/>
@@ -42481,7 +42499,7 @@
       <c r="M48" s="92"/>
       <c r="N48" s="115"/>
       <c r="O48" s="92" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="P48" s="92"/>
       <c r="Q48" s="92"/>
@@ -42534,7 +42552,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="59" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F49" s="62"/>
       <c r="G49" s="62"/>
@@ -42546,7 +42564,7 @@
       <c r="M49" s="62"/>
       <c r="N49" s="116"/>
       <c r="O49" s="62" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="P49" s="62"/>
       <c r="Q49" s="62"/>
@@ -42655,7 +42673,7 @@
       <c r="B51" s="60"/>
       <c r="C51" s="61"/>
       <c r="D51" s="62" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E51" s="65"/>
       <c r="F51" s="65"/>
@@ -44310,7 +44328,7 @@
       <c r="C79" s="50"/>
       <c r="D79" s="62"/>
       <c r="E79" s="50" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F79" s="50"/>
       <c r="G79" s="50"/>
@@ -44430,7 +44448,7 @@
       <c r="C81" s="50"/>
       <c r="D81" s="62"/>
       <c r="E81" s="61" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="F81" s="62"/>
       <c r="G81" s="63"/>
@@ -44492,7 +44510,7 @@
       <c r="D82" s="62"/>
       <c r="E82" s="61"/>
       <c r="F82" s="62" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="G82" s="63"/>
       <c r="H82" s="62"/>
@@ -44612,7 +44630,7 @@
       <c r="D84" s="62"/>
       <c r="E84" s="61"/>
       <c r="F84" s="62" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="G84" s="187"/>
       <c r="H84" s="188"/>
@@ -44674,7 +44692,7 @@
       <c r="E85" s="61"/>
       <c r="F85" s="62"/>
       <c r="G85" s="67" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H85" s="68"/>
       <c r="I85" s="68"/>
@@ -44683,7 +44701,7 @@
       <c r="L85" s="68"/>
       <c r="M85" s="199"/>
       <c r="N85" s="200" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="O85" s="201"/>
       <c r="P85" s="201"/>
@@ -44746,7 +44764,7 @@
       <c r="L86" s="190"/>
       <c r="M86" s="202"/>
       <c r="N86" s="203" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="O86" s="204"/>
       <c r="P86" s="204"/>
@@ -45095,7 +45113,7 @@
       <c r="E92" s="61"/>
       <c r="F92" s="64"/>
       <c r="G92" s="67" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H92" s="68"/>
       <c r="I92" s="68"/>
@@ -45104,7 +45122,7 @@
       <c r="L92" s="68"/>
       <c r="M92" s="199"/>
       <c r="N92" s="200" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="O92" s="201"/>
       <c r="P92" s="201"/>
@@ -45158,7 +45176,7 @@
       <c r="E93" s="61"/>
       <c r="F93" s="64"/>
       <c r="G93" s="189" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="H93" s="190"/>
       <c r="I93" s="190"/>
@@ -45167,7 +45185,7 @@
       <c r="L93" s="190"/>
       <c r="M93" s="202"/>
       <c r="N93" s="203" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="O93" s="204"/>
       <c r="P93" s="204"/>
@@ -45516,7 +45534,7 @@
       <c r="E99" s="61"/>
       <c r="F99" s="64"/>
       <c r="G99" s="67" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H99" s="68"/>
       <c r="I99" s="68"/>
@@ -45525,7 +45543,7 @@
       <c r="L99" s="68"/>
       <c r="M99" s="199"/>
       <c r="N99" s="200" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="O99" s="201"/>
       <c r="P99" s="201"/>
@@ -45579,7 +45597,7 @@
       <c r="E100" s="61"/>
       <c r="F100" s="64"/>
       <c r="G100" s="189" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="H100" s="190"/>
       <c r="I100" s="190"/>
@@ -45588,7 +45606,7 @@
       <c r="L100" s="190"/>
       <c r="M100" s="202"/>
       <c r="N100" s="203" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="O100" s="204"/>
       <c r="P100" s="204"/>
@@ -45937,7 +45955,7 @@
       <c r="E106" s="61"/>
       <c r="F106" s="64"/>
       <c r="G106" s="67" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H106" s="68"/>
       <c r="I106" s="68"/>
@@ -45946,7 +45964,7 @@
       <c r="L106" s="68"/>
       <c r="M106" s="199"/>
       <c r="N106" s="200" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="O106" s="201"/>
       <c r="P106" s="201"/>
@@ -46000,7 +46018,7 @@
       <c r="E107" s="61"/>
       <c r="F107" s="64"/>
       <c r="G107" s="189" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="H107" s="190"/>
       <c r="I107" s="190"/>
@@ -46009,7 +46027,7 @@
       <c r="L107" s="190"/>
       <c r="M107" s="202"/>
       <c r="N107" s="203" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="O107" s="204"/>
       <c r="P107" s="204"/>
@@ -46358,7 +46376,7 @@
       <c r="E113" s="61"/>
       <c r="F113" s="64"/>
       <c r="G113" s="67" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H113" s="68"/>
       <c r="I113" s="68"/>
@@ -46367,7 +46385,7 @@
       <c r="L113" s="68"/>
       <c r="M113" s="199"/>
       <c r="N113" s="200" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="O113" s="201"/>
       <c r="P113" s="201"/>
@@ -46421,7 +46439,7 @@
       <c r="E114" s="61"/>
       <c r="F114" s="64"/>
       <c r="G114" s="189" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="H114" s="190"/>
       <c r="I114" s="190"/>
@@ -46430,7 +46448,7 @@
       <c r="L114" s="190"/>
       <c r="M114" s="202"/>
       <c r="N114" s="203" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="O114" s="204"/>
       <c r="P114" s="204"/>
@@ -46779,7 +46797,7 @@
       <c r="E120" s="61"/>
       <c r="F120" s="64"/>
       <c r="G120" s="67" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H120" s="68"/>
       <c r="I120" s="68"/>
@@ -46788,7 +46806,7 @@
       <c r="L120" s="68"/>
       <c r="M120" s="199"/>
       <c r="N120" s="200" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="O120" s="201"/>
       <c r="P120" s="201"/>
@@ -46842,7 +46860,7 @@
       <c r="E121" s="61"/>
       <c r="F121" s="64"/>
       <c r="G121" s="189" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="H121" s="190"/>
       <c r="I121" s="190"/>
@@ -46851,7 +46869,7 @@
       <c r="L121" s="190"/>
       <c r="M121" s="202"/>
       <c r="N121" s="203" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="O121" s="204"/>
       <c r="P121" s="204"/>
@@ -47142,7 +47160,7 @@
       <c r="F126" s="64"/>
       <c r="G126" s="64"/>
       <c r="H126" s="583" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="I126" s="171"/>
       <c r="J126" s="171"/>
@@ -47203,7 +47221,7 @@
       <c r="F127" s="64"/>
       <c r="G127" s="195"/>
       <c r="H127" s="583" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="I127" s="171"/>
       <c r="J127" s="171"/>
@@ -47263,13 +47281,13 @@
       <c r="E128" s="61"/>
       <c r="F128" s="64"/>
       <c r="G128" s="196" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="H128" s="197"/>
       <c r="I128" s="197"/>
       <c r="J128" s="211"/>
       <c r="K128" s="67" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="L128" s="68"/>
       <c r="M128" s="68"/>
@@ -47298,7 +47316,7 @@
       <c r="AJ128" s="68"/>
       <c r="AK128" s="199"/>
       <c r="AL128" s="67" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="AM128" s="68"/>
       <c r="AN128" s="68"/>
@@ -47328,13 +47346,13 @@
       <c r="E129" s="61"/>
       <c r="F129" s="64"/>
       <c r="G129" s="218" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="H129" s="219"/>
       <c r="I129" s="219"/>
       <c r="J129" s="224"/>
       <c r="K129" s="225" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="L129" s="226"/>
       <c r="M129" s="226"/>
@@ -47363,7 +47381,7 @@
       <c r="AJ129" s="226"/>
       <c r="AK129" s="233"/>
       <c r="AL129" s="234" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="AM129" s="226"/>
       <c r="AN129" s="226"/>
@@ -47377,7 +47395,7 @@
       <c r="AV129" s="233"/>
       <c r="AW129" s="171"/>
       <c r="AY129" s="240" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="AZ129" s="240"/>
       <c r="BA129" s="240"/>
@@ -47395,13 +47413,13 @@
       <c r="E130" s="61"/>
       <c r="F130" s="64"/>
       <c r="G130" s="220" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="H130" s="221"/>
       <c r="I130" s="221"/>
       <c r="J130" s="227"/>
       <c r="K130" s="228" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="L130" s="171"/>
       <c r="M130" s="171"/>
@@ -47430,7 +47448,7 @@
       <c r="AJ130" s="171"/>
       <c r="AK130" s="235"/>
       <c r="AL130" s="236" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="AM130" s="171"/>
       <c r="AN130" s="171"/>
@@ -47444,7 +47462,7 @@
       <c r="AV130" s="235"/>
       <c r="AW130" s="171"/>
       <c r="AY130" s="240" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="AZ130" s="240"/>
       <c r="BA130" s="240"/>
@@ -47462,13 +47480,13 @@
       <c r="E131" s="61"/>
       <c r="F131" s="64"/>
       <c r="G131" s="222" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="H131" s="223"/>
       <c r="I131" s="223"/>
       <c r="J131" s="229"/>
       <c r="K131" s="230" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="L131" s="231"/>
       <c r="M131" s="231"/>
@@ -47497,7 +47515,7 @@
       <c r="AJ131" s="231"/>
       <c r="AK131" s="238"/>
       <c r="AL131" s="239" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="AM131" s="231"/>
       <c r="AN131" s="231"/>
@@ -47511,7 +47529,7 @@
       <c r="AV131" s="238"/>
       <c r="AW131" s="171"/>
       <c r="AY131" s="240" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="AZ131" s="240"/>
       <c r="BA131" s="240"/>
@@ -47704,7 +47722,7 @@
       <c r="B135" s="60"/>
       <c r="C135" s="50"/>
       <c r="D135" s="581" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E135" s="50"/>
       <c r="F135" s="50"/>
@@ -49417,7 +49435,7 @@
       <c r="B164" s="60"/>
       <c r="C164" s="50"/>
       <c r="D164" s="62" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E164" s="50"/>
       <c r="F164" s="50"/>
@@ -49475,7 +49493,7 @@
     </row>
     <row r="165" customHeight="1" spans="4:4">
       <c r="D165" s="62" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="167" customHeight="1" spans="4:48">
@@ -49654,7 +49672,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="13"/>
       <c r="J1" s="14" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
@@ -49662,7 +49680,7 @@
       <c r="N1" s="15"/>
       <c r="O1" s="16"/>
       <c r="P1" s="14" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="Q1" s="15"/>
       <c r="R1" s="15"/>
@@ -49670,14 +49688,14 @@
       <c r="T1" s="15"/>
       <c r="U1" s="16"/>
       <c r="V1" s="21" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="W1" s="22"/>
       <c r="X1" s="22"/>
       <c r="Y1" s="22"/>
       <c r="Z1" s="25"/>
       <c r="AA1" s="26" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="AB1" s="15"/>
       <c r="AC1" s="15"/>
@@ -49691,20 +49709,20 @@
       <c r="AK1" s="15"/>
       <c r="AL1" s="16"/>
       <c r="AM1" s="29" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="AN1" s="30"/>
       <c r="AO1" s="33" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="AP1" s="34"/>
       <c r="AQ1" s="35"/>
       <c r="AR1" s="36" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="AS1" s="30"/>
       <c r="AT1" s="37" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="AU1" s="38"/>
       <c r="AV1" s="38"/>
@@ -49750,20 +49768,20 @@
       <c r="AK2" s="19"/>
       <c r="AL2" s="20"/>
       <c r="AM2" s="31" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="AN2" s="32"/>
       <c r="AO2" s="39" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="AP2" s="40"/>
       <c r="AQ2" s="41"/>
       <c r="AR2" s="31" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="AS2" s="32"/>
       <c r="AT2" s="42" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
       <c r="AU2" s="43"/>
       <c r="AV2" s="43"/>
@@ -49823,7 +49841,7 @@
     <row r="4" s="2" customFormat="1" spans="1:49">
       <c r="A4" s="9"/>
       <c r="B4" s="10" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>

</xml_diff>